<commit_message>
fix: minor alignment fixes
</commit_message>
<xml_diff>
--- a/accessdb/templateSheets/01defFamSheet.xlsx
+++ b/accessdb/templateSheets/01defFamSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\win11vm\networkdb\Registry\defFamSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jovial\Documents\Workspace\GitHub\cbcef-frdb\accessdb\templateSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34233B9-D2A3-4EB1-B0BB-ED854F00859F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADE1703-8485-4F75-B574-F796F1E94A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{691864EF-CD39-4A4F-A743-1915A8367D6B}"/>
   </bookViews>
@@ -1343,9 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B0EA35-602C-4E1F-A94E-665F1CEBDA8B}">
   <dimension ref="A1:C1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
fix: adds proper intent & minor fix
</commit_message>
<xml_diff>
--- a/accessdb/templateSheets/01defFamSheet.xlsx
+++ b/accessdb/templateSheets/01defFamSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jovial\Documents\Workspace\GitHub\cbcef-frdb\accessdb\templateSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\win11vm\networkdb\Registry\defFamSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADE1703-8485-4F75-B574-F796F1E94A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B408DE92-1CC6-45A7-A9E3-42EFCFD3EAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{691864EF-CD39-4A4F-A743-1915A8367D6B}"/>
   </bookViews>
@@ -269,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -319,12 +319,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
@@ -345,6 +339,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,12 +379,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -394,13 +398,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1037,7 +1040,7 @@
   <autoFilter ref="A5:C48" xr:uid="{7ED75F74-C5D4-4B51-8775-6C43A3A144B1}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6D668163-801A-41BB-B009-B9F1EBB13689}" name="Sl. No." totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{BF741685-7980-46D2-B60C-07F0984CB8EA}" name="Description" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BF741685-7980-46D2-B60C-07F0984CB8EA}" name="Description" dataDxfId="1" totalsRowDxfId="2"/>
     <tableColumn id="3" xr3:uid="{F4DDDD5A-3EBA-47E6-A236-E0C7A8103AA5}" name="Member 1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1343,7 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B0EA35-602C-4E1F-A94E-665F1CEBDA8B}">
   <dimension ref="A1:C1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1370,13 +1375,13 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1387,7 +1392,7 @@
       <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
@@ -1396,7 +1401,7 @@
       <c r="B7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
@@ -1405,7 +1410,7 @@
       <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
@@ -1414,7 +1419,7 @@
       <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="25"/>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
@@ -1423,7 +1428,7 @@
       <c r="B10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
@@ -1432,7 +1437,7 @@
       <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="25"/>
     </row>
     <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
@@ -1441,7 +1446,7 @@
       <c r="B12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="25"/>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
@@ -1450,7 +1455,7 @@
       <c r="B13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
@@ -1459,7 +1464,7 @@
       <c r="B14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="24"/>
     </row>
     <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
@@ -1468,7 +1473,7 @@
       <c r="B15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
@@ -1477,7 +1482,7 @@
       <c r="B16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
@@ -1486,7 +1491,7 @@
       <c r="B17" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
@@ -1495,7 +1500,7 @@
       <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
@@ -1504,7 +1509,7 @@
       <c r="B19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
@@ -1513,7 +1518,7 @@
       <c r="B20" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
@@ -1522,56 +1527,56 @@
       <c r="B21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="24"/>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="24"/>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="24"/>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="24"/>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="24"/>
     </row>
     <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="24"/>
     </row>
     <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="24"/>
     </row>
     <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15">
@@ -1580,16 +1585,16 @@
       <c r="B29" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="24"/>
     </row>
     <row r="30" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15">
         <v>18</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="24"/>
     </row>
     <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15">
@@ -1598,137 +1603,137 @@
       <c r="B31" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="24"/>
     </row>
     <row r="32" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <v>20</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="24"/>
     </row>
     <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
+      <c r="C33" s="24"/>
     </row>
     <row r="34" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <v>21</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="24"/>
     </row>
     <row r="35" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <v>22</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="17"/>
+      <c r="C35" s="24"/>
     </row>
     <row r="36" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15">
         <v>23</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="24"/>
     </row>
     <row r="37" spans="1:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <v>24</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="24"/>
     </row>
     <row r="38" spans="1:3" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <v>25</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="24"/>
     </row>
     <row r="39" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <v>26</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="24"/>
     </row>
     <row r="40" spans="1:3" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <v>27</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="24"/>
     </row>
     <row r="41" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15">
         <v>28</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="24"/>
     </row>
     <row r="42" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15"/>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="24"/>
     </row>
     <row r="43" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15"/>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="24"/>
     </row>
     <row r="44" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="24"/>
     </row>
     <row r="46" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="24"/>
     </row>
     <row r="47" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15">
         <v>29</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="24"/>
     </row>
     <row r="48" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15">
@@ -1737,7 +1742,7 @@
       <c r="B48" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="24"/>
     </row>
     <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
@@ -1745,45 +1750,45 @@
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23"/>
+      <c r="A51" s="21"/>
       <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="7"/>
     </row>
     <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="9"/>
     </row>
     <row r="56" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
+      <c r="A56" s="22"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9"/>
     </row>

</xml_diff>